<commit_message>
Added overall Sentiment from Google API and google entities, however they prove chaotic and we will need to see if we keep them or not
</commit_message>
<xml_diff>
--- a/songlyrics_cat.xlsx
+++ b/songlyrics_cat.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hytiroglou Dimitris\Desktop\Readings\Info 202 - Information Organization &amp; Retrieval\Project\motif\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="860">
   <si>
     <t>ID</t>
   </si>
@@ -2219,13 +2224,388 @@
   </si>
   <si>
     <t>['Wu-Tang Clan', 'Hip hop music', 'Culture', 'Religious belief and doctrine', 'Religion', 'Religious behaviour and experience', 'Literature', 'Hip hop', 'Shacharit for Shabbat and Yom Tov', 'Shabbat prayers']</t>
+  </si>
+  <si>
+    <t>overall_sentiment</t>
+  </si>
+  <si>
+    <t>Janie,honey,Dum,sound,dog day,gun,run,honey,Dum,gun,pain,gun,Honey,sleaze,Yeah,gun,gun,gun,gun,daddy,world,everybody,run,man,gun,everybody,run,lookin,train,sun,man,dog day,gun,gun,pain,daddy,daddy,everybody,Cause Janie,someone,man,gun,gun,thunder,baby,lightnin,brain,bullet,everybody,gun Everybody,gun,gun,gun,problem,spell,daddy,I.O.U.,cradle robbin,nobody</t>
+  </si>
+  <si>
+    <t>fire burnin,Cause,doctor,doctor,rocker,rocker,shove,love,Somebody,fool child,shotgun,message,magic touch,way,babe,habit,child,babe,magic touch,shotgun,surprise,fire,wedding,burnin,habit,magic touch,fire,babe,Gonna,magic touch</t>
+  </si>
+  <si>
+    <t>kind,taste,Gotta,tongue,tip,beat,India,Taste Of India,God,taste,taste,tongue,tip,face,taste,taste,cat man,friend,love incense,back room,funk,perfume,darkness,tongue,tip,stuff,smile,cat man,love,shadow,light,thing,vindaloo,heart,fire,priestess,bliss,delight,love,Yin and Yang,shadow,taste,mine,cat man,smile,face,taste,appetite,smile,friend,appetite,mine,Yow,concubine,wine</t>
+  </si>
+  <si>
+    <t>Lord,Everybody,face,past,mirror,dusk,way,lines,sin,Sing,Lord,life,everybody,Sing,laughter,tear,things,Lord,books,laughter,tear,Sing,life,dues,pages,sages,fools,tear,laughter,dreams,dreams,Sing,Dream on Dream on Dream on Dream,Dream on Dream on Dream on Dream on Dream on Dream on Dream on Sing,laughter,tear</t>
+  </si>
+  <si>
+    <t>girl,woman,millionaire,baby,Lordy,god,god,Lord,Man,blind,eyesight,millionaire,way,way,state,cause,bed,head,back room,cause,blind,eyesight,eyes,Man,blind,eyesight,woman</t>
+  </si>
+  <si>
+    <t>way,man,hands,pockets,offI,promise,things,time,Intentions,mind,heart,thinkI,number,wall,best,eyes,ears,stoneI,Beginning,callI,excuse,back,saidI,offMy,I fallI,tallI,thinkIs</t>
+  </si>
+  <si>
+    <t>child,one,misery,thinking,baby,Cause,mama,everything,style,baby,baby,But,baby,baby,Yeah,baby,baby,ride,velvet glove,side,Yeah,baby,ecstasy,baby,breeze,Love</t>
+  </si>
+  <si>
+    <t>greed Maidens,lords,bishops,gold,wombs,knights,Were,Starch,lives,all,queens,guillotines,parchment,laws,swords,ride,turnin,Truths,nightmares,Dreams,life,Screams,Sailing ships,father,blood,land,Kings,Tossin,Viking,reply,Screams,reply,Deja vu,Died Lordy,maidens,swords,loss,pride,death,mares,times,Sneer</t>
+  </si>
+  <si>
+    <t>lid,Boys,cops,street,rival,word,avenue,streets gang clash,heads,lightning,eye,Gonna,lightning strikes,Blades,finger,hell's kitchen,gun,lightning strikes,funeral rights,street,thunder,all,ones,chains,parking lot,tooth,tooth,blood,Gotta,heat,street,combat zone,means,dog eat dog,Johnny,Zip,thunder,cops,ones,chains,funeral rights,blood,heat,lightning strikes,licks,Lightning,lightning strikes,lightning strikes,lightning strikes,lightning strikes,parking lot,all,dagger knife,suicide blitz,thunder</t>
+  </si>
+  <si>
+    <t>something,advice,luck,Keep,rollerskates,Try,ball,ball,ball,Try,air,rowing,boat,hands,end,toes,chin,belly,nose,head,top,floor,Try,grooving,no,no,no,trip,tip</t>
+  </si>
+  <si>
+    <t>baby,lot,morphine,religion,door,medication,same,Ooh,baby,door,mind,sunlight,skies,side,floor,matter,sacrifices,knees,Ooh,clouds,eyes,same,pieces,minds,shoes,guy,girl,thing,mother,daddy,something,darlin,baby,pieces,skies,sunlight,same,Cause,clouds,eyes,Walkin,baby,skies,sunlight,eyes,clouds</t>
+  </si>
+  <si>
+    <t>pain,sorrow,world,greetings,job,place,place,shot,liquor store,beer,top,pores,way,Lotto tickets,Tryna,shot,Whiskey,block,nowhere,liquor store blues,shot,sorrow,drag,drag,drag,thing,block,nowhere,liquor store blues,city lights,guitar,rent,cops,pineapple kush,thing,Tryna,shot,jaws,greetings,world,shot,Superman,Cause,Junior Gong</t>
+  </si>
+  <si>
+    <t>first,bed,man,pride,ooh ooh hoo hoo Mm,hand,friends,cause,cause,baby,same,chance,bit,heart,radio,song,flowers,name,hand,dancing,man,chance,party,ooh,flowers,ways,mess,life,woman,needs,ego,eyes,flowers,dancing,man,party,baby,mistakes,things,things,chance,party</t>
+  </si>
+  <si>
+    <t>love,liquor,cocaine Kicker,sky,devil,eyes,legs,bottle,baby,neighbors,daddy,love,baby,baby,gorilla,gorillas,gorillas,jungle,lover,killer,Bang bang,chest,hair,cops,sheriff,swat,door,body,fistful,baby,baby,gorillas,killer,Bang bang,baby,gorillas,baby,gorillas,gorillas,baby,chest,jungle,gorilla Ooh,gorillas,baby</t>
+  </si>
+  <si>
+    <t>Right,eyes,body,need,woman,lips,way,eyes,way,mind,way,Baby,need,boom boom boom,pleasure island,waste,boom boom boom,bus,Girl,girl,room room room,zoom zoom Baby,zoom zoom Baby,Darling,room room room</t>
+  </si>
+  <si>
+    <t>girls,death,death,girls,Guess,birds,sun,roads,car,money,name,hunnies,girls,Boy meets girl,girls,girls,girls,death,matter,matter,mess,everything,roads,wife,love,lies,words,lights,mess,Start,matter,matter,mess,wild,matter,matter</t>
+  </si>
+  <si>
+    <t>best,face,tears,something,reverse,someone,waste,Tears,Lights,bones,Lights,love,Tears,mistakes,bones,Tears,something,Tears,bones,I Lights</t>
+  </si>
+  <si>
+    <t>fool mess,thing,sky A star,Everyone,Everyone,love,call,sun,stomach,Everyone,eyes,Everyone,thing,star,love,call,cage,cage,line</t>
+  </si>
+  <si>
+    <t>eyes,Oh,words,angels,blossom,beauty,eyes,eyes,Eyes,storm,lightning,blossom,puddles,dirt,stars,world,miracles,world,eyes,storm,lightning,Believe</t>
+  </si>
+  <si>
+    <t>refuge,thing,baby,power,baby,sea,sky,power,Moses,air,air,somewhere,opportunity,difference,matter,II,sky,Oh</t>
+  </si>
+  <si>
+    <t>one,sea,tree,shelf,eyes,song,sea,book,sea,darling,size,line,world,good,nothing,streets,Forget,streets,houses,song,houses</t>
+  </si>
+  <si>
+    <t>king,world,word,streets,word,mirror,missionaries,bells,Seas,eyes,enemy,crowd,dice,fear,Oh,world,pillars,choirs,pillars,sword,field,reason,Jerusalem,windows,wind,sand,key,castles,salt,walls,doors,sound,drums,reason,field,sword,choirs,Chorus,world,Roman Cavalry,People,name,king,Roman,Calvary,string,puppet,silver plate,head,Revolutionaries,Saint Peter,Oh</t>
+  </si>
+  <si>
+    <t>boy,Part,Everything,system,shadows,human race,em,something,part,Part,space,sound,system plan,noise,state,state,Things,shadows sparkle,state,All,Part,outer space,space,Everything,system plan,noise,state,stars,state,state Swimming,sea,faces,tide,answer,sun,horizon,love</t>
+  </si>
+  <si>
+    <t>thing,everything,stars,song,Look,things,turn,thing,skin,skin,thing,skin,skin,something,bones,line,line,things,stars,bones,something</t>
+  </si>
+  <si>
+    <t>heart beating,Honey,gravity,everyone,sound,sun,way,gravity,sun,way,Oh,everyone,sky,sun,way,gravity,sun,way,gravity,sky,sound</t>
+  </si>
+  <si>
+    <t>drink,drink,angel,world,drug,Life,Oh,symphony,river,wings,I,drink,flood,wings,symphony,wings,wings,stars,symphony,angel,Life,love,blood,I,I,lalalala,sky,sky,sky,sky</t>
+  </si>
+  <si>
+    <t>all,tattoo,all,life,name,pocket knife,All,Feels,All,something,All,way,pains,tattoo,stars,colors,thirst,Oh,All,road,fire</t>
+  </si>
+  <si>
+    <t>creatures,house,garden,Love Street She,store,Love Street,wisdom,flunkies,monkeys,robes,La,la,la,la,wisdom,la,la,La,Love Street There,la,garden,house</t>
+  </si>
+  <si>
+    <t>someone,trip,ribbons,hair,rain,FM set,people,window,sister,world,lovers,friend,window,baby,fire,Well,road,door,phone,heart ache,valley,lake,grass,guitars,musicians,Yeah,Yeah,everything,farm,mountains,car,diamonds,mother,father,home,Chicago</t>
+  </si>
+  <si>
+    <t>Crawlin' King Snake,Gonna,den,den,Seein,baby,round,Ooo,den,baby,crawl,C'mon,Grass,den,everything,floor,C'mon crawl C'mon crawl,den,Ai,round,mate,baby,Crawl,spider,knees,hands</t>
+  </si>
+  <si>
+    <t>end,highway,End,journey,Some,Some,Some,delight,realms,delight,Realms,End,light,bliss,Some,delight,Some,Some,Realms,realms,delight,bliss,light</t>
+  </si>
+  <si>
+    <t>liar,liar,fire,fire,fire,love,baby,baby,Girl,fire,fire,fire,fire,baby,baby,baby,baby,mire Try,fire,fire,mire Try,funeral pyre,funeral pyre,love,baby,baby,fire,fire,fire,fire,fire,fire</t>
+  </si>
+  <si>
+    <t>ways,Yeah,daddy,face,love,love,love,love,love,door,door,love,love,song,horses,dream,ways,song,horses,dream,mark,love,love,door</t>
+  </si>
+  <si>
+    <t>one,web,captives,pearl,friendship,knots,Crystal,jewel,fight,friend,Crystal,Crystal,Crystal,oyster,world,distance,care,run,end,truth,heart,peace,cells,bars,Crystal,girl</t>
+  </si>
+  <si>
+    <t>mirror,silver spoon,sun,birds,snow,poem,songs,drink,hand,wine,land,lambs,moon,page</t>
+  </si>
+  <si>
+    <t>pulse,hoop,fire,lips,things,dreams,walks,beaches,guitars,nylon strings,reads,reads,reads,reads,fire,hoop,heat,wealth,mistrust,fire,hoop,fire,hoop,hoop,fire,pulse,love,fire,hoop,nights,strangers,pressure,places,hoop,fire,hoop,fire,hoop,fire,hoop,fire,hoop,fire</t>
+  </si>
+  <si>
+    <t>nothing,hill,house,house,home,bones,brick,girl,home,home,piece,piece,bit,Bit,brick,brick,cards,brick,brick,skin,teeth,girl,lot,someone,house,Build,someone,home,friends,passion,Build,spades,spades,cards,brick,hearts,cars,table,schemes,house,lot,grave,home,Build,home,girl,home,girl,house,lot,someone,someone,lot</t>
+  </si>
+  <si>
+    <t>moon,chieftain,sons,Oh,moon,wood smoke,warlance,warlord,sun,hills,woman,tepee,smell,cobweb,ones,land,father,soldiers,guns,buzzards,reason,writing,pony,man,chieftain,sound,smoke,fathers,gold,pony wild,drums,tomahawk,breast,child,squaw,man fears,words,race,daughter,kind,pride,healing waters,prairie,tribe,Geronimo,Iroquois,Lord,hoof tracks,Sioux,Yellow Dog,home,gauntlet,horse soldiers,running,bow,peace,sand,hands,weapons,loved ones,sound,guns,gold,buffaloes,clover fields,warrior,bullet hole,lead,renegades</t>
+  </si>
+  <si>
+    <t>Chesay Chesay,luck,devil,Magic,drink,Chesay,shame,luck,gypsy way,things,Chesay,nothing,star,cup,gypsy love,Chesay Swallow,luck,luck,luck,drink,devil,Magic</t>
+  </si>
+  <si>
+    <t>baby,Turn,Dig,everybody,bongo sound,one,reach,clam,clam,clam,hand,tease,clam,clam,clam,beach,baby,hand,tease,heart,Everybody,outside,appetite,clam,clam,beat,clam,clam,Moon,clam,hand,tease,clam Dig,hand,tease,clam,clam</t>
+  </si>
+  <si>
+    <t>Angel,street Earth,angel,earth boy,boy dream,All,earth boy,land,heart,earth boy,dream,dreams,earth boy,land,boy,boy,angel,sun,love,land,doves,story,part,All,walk,love,Oo-oo-oo,earth boy,earth boy,angel,dream,boy dream,dream,boy dream,dreams,part,land,story,doves</t>
+  </si>
+  <si>
+    <t>Drivin,toodle-loo,number,blues,place,good-bye,No,advice,luck,luck,remembering,Black cats,woe,tree,money,kind,luck,luck,mind,luck,way,blues,luck,knee,thing,lady luck,luck,losers,everything,decks,Yes,hex</t>
+  </si>
+  <si>
+    <t>sight,guys,love,girl,heart,heart,ground,town,double trouble,trouble,anybody,trouble,matchbox,sea,cards,clouds,grade</t>
+  </si>
+  <si>
+    <t>feeling,pillow,moonlight,hair,hand,girl,mine,love,girl,sleeping lips,smile,girl,Eyes,life,road,clouds,sea,arms,love,love,girl,things,girl,Eyes,clouds,sea,light,mine,arms,road,life,love,girl,light,mine,smile</t>
+  </si>
+  <si>
+    <t>love,girl,things,twinkle,arms,love,girl,eyes</t>
+  </si>
+  <si>
+    <t>speed,mind,train,cocaine,Trouble,trouble,Trouble,Casey Jones,bout,Trouble,notion,end,engine,trouble,train,cocaine,notion,advice,sleeping,Leaves Central Station,notion,Hits River Junction,Lady,Switchman,engine,trouble,eyes,bend,fireman screams,two,cocaine,train,track</t>
+  </si>
+  <si>
+    <t>mama,home,airplane,Calamity,style,avenue,Truckin,Cosmic Charlie,Rosey,Dum de dum de do da lee,Calico Cal,ones,blue,paper canoe,way,paddle,last,first,mama,waiting,first,wind,Cat,Everything,bit,old ones,home,Mama,seaside zoo,mama,mama,home,home,home,Calliope,word,last,people</t>
+  </si>
+  <si>
+    <t>nightfall,Dark star crashes,ashes,light,Reason tatters,axis,forces,casting,diamonds,faults,clouds,delusion,reflections,matter,hand,Searchlight,nights,goodbye,Mirror,diamonds,petal flowers,velvet,Lady</t>
+  </si>
+  <si>
+    <t>eyes,Wonderin,eyes,tree,girl,Gypsy Way,country side,world,gypsy eyes,one,eyes,road,rubble road side,girl,some,love,tears,tryin,death,getaway,men,Gypsy Well,road,side,eyes,battle,worry knees,time,call,Lord,highway</t>
+  </si>
+  <si>
+    <t>traffic,speed,car,girl,front,side,soul,pain,ride,town,hit and run,back,traffic jam,fun,signals,green,town,baby,Tire,street,darling,things,Crosstown</t>
+  </si>
+  <si>
+    <t>baby,love,man,love,speed,lot,find,lover,man,Mmm,Whoo,fool baby,woman,Come,chain,pain,life,man,Everybody,Doodoo doodoo,eyes,baby,Everybody,Yeah,Hey Come on baby Come on Come on Fly,Hey Yeah,talent Work,mind</t>
+  </si>
+  <si>
+    <t>something,baby,Lord,house,yonder,baby,baby,house,Something,something,something,baby,home,baby,lord,Lord,Lord,key,door,mercy,door,feeling,yonder,Way,hill,Cause,sister,yonder,hill,Yeah</t>
+  </si>
+  <si>
+    <t>reason,buddy miles,something,mind,mind,mind,baby,some,Yeah,everybody,mind,baby,fun,crime,hands,hands,Ooo hooo Well,some,love,Whaa,Everything goin</t>
+  </si>
+  <si>
+    <t>Lord,Lord,voodoo child baby,mountain,edge,hand,Yeah Well,Yeah,thing,mountain,edge,hand,one,pieces,island,Cause,no,answer Question,world,one</t>
+  </si>
+  <si>
+    <t>Things,Things,end,words,Heaven,chance,mind,thing,things,hand,secrets,end,beat,repeat,words,touch,dance,sound,control,Let,So,repeat,hands,Baby,ground,romance,moment,way,beat,Heaven,love</t>
+  </si>
+  <si>
+    <t>elevator,trouble,TV crews,shit,penthouse floor,news,city lights,folks,baby,truth,lies,sky,order,Streets,show,penthouse floor,penthouse floor,Penthouse floor,elevator,future,penthouse,penthouse floor,penthouse floor,Penthouse floor,times,notice,man,penthouse,penthouse floor,penthouse floor,altitude,holding,joke,city lights,more,rooms,Oh,home,babe,knock,patience,view,line,song,phone,hair,apples,eggs,Conversations,dress,crab legs,penthouse floor,penthouse floor,penthouse floor,party,penthouse babe,mix,bliss,ignorance,Jump,elevator,Baby,penthouse doors,penthouse doors,penthouse doors,Baby,jokes,news,folks,group,suit,smile,boy,trunk,top,clouds,room,Til,Forcin</t>
+  </si>
+  <si>
+    <t>Alright,Cuz,storm,heaven,angel,life,clouds,sun,doubt,Friends,need,war,Storms,winds,rise,friends,love,peace,Oooh,life,peace,need,need,struggle,place,Baby,grace,mind,storm,battles,love,Israel There,faith,eyes,peace,storm,Baghdad,Ooh,peace,middle,Alright,Alright,storm,love,peace</t>
+  </si>
+  <si>
+    <t>cast,case,face,light,stars,prisoners,history,minds,sparks,life,miracles,flame,line,name,clouds,distance,space,people,hero,light</t>
+  </si>
+  <si>
+    <t>things,heaven,sleep,something,talk,sign,watchin,Show,Life,reality,mystery,meaning,all,light,thanks,suffering,mercy,peace,love,price,way,world,people,life,Oh God,nme</t>
+  </si>
+  <si>
+    <t>do,do,thing,Baby,thing,mama,home,cold,fame,mind,dr,dream,class,soul,All,All,song,King,teacher,All,All,mind,wife,temptress,Everybody,front,crowd,spell,well,tricks,niggas,somebody,somebody,many,people,whatever,lane,lane,Tryna</t>
+  </si>
+  <si>
+    <t>folks,no one,Legend,baby,door,things,Things,truth,lie,kings,door,love,lack,nothing,light,fame,door,floor,music,power,place,color,face,history</t>
+  </si>
+  <si>
+    <t>friends,Bridges,money,brother,visions,luxury,Whatcha,Nowhere,nowhere,no one,world,Nowhere,money,pursuit,peace,reality,dough,search,life,soul,Nowhere,nowhere,joy,beast,American Dream,Hey Whatcha,Whatcha,Nowhere,nowhere,Nowhere,nowhere</t>
+  </si>
+  <si>
+    <t>name,name,man,man,man,man,love,love,name,love,more,Shot rings,love,more,love,love,love,love,love,man,more,man,more,love,love,love,more,beach,fence,kiss,love,love,love,love,sky,more,more,love,Memphis,more,pride,life</t>
+  </si>
+  <si>
+    <t>hocus pocus,spell,wonder wonder,satisfaction,eyes,wonder wonder,way,focus,kiss,Repeat,satisfaction,much,magic pass,love,love,love,cold shoulder</t>
+  </si>
+  <si>
+    <t>hit,dance,Got,Da-da-doo-doo,bit,Red wine,dance,All,drink,keys,hit,tryin,Konvict,Gaga,floor,record baby,people,man,phone,just dance spin,dance,dance,dance,Just dance,Shawty,dance,dance,record babe,dance,Da da doo doo,dance,name,club,Chorus,record babe,floor,playboy mouth,record baby,da-da-doo-doo,club,name,Chorus,dance,dance,dance,dance,reason,thorns,dance floor checkin,catalog,flaw,women,eyes,car,blueprint,blueprint,hips,round,meantime stand,poison babe Roses,Half,record babe,record babe,Just dance,dance,dance,dance,muscle,hustle,dough,pocko,energy,Gonna,shirt,way,record babe,blueprint,Lysol,Go,Half</t>
+  </si>
+  <si>
+    <t>Town,sound,Anybody,hand,anybody,sound,black light,Baby,trick,forest land,back room,Honey,eyes,sound,anybody,honey,love,rock show,smile,sound,visions,light,place,house,window,freakshow,anybody,eyes,love,Baby,girl,Uh,rock show,rock show Rock show,rock show,rock show</t>
+  </si>
+  <si>
+    <t>love,romance,Rah rah ah-ah-ah!,bitch baby,revenge,Ro,ro-mah-mah Gaga ooh,love,love,Walk,romance,la-la,la-la,lovers revenge,love,love,love,romance,romance,romance,romance,love,love,romance,romance,romance,romance,design,ro-mah-mah Gaga,la-la,romance,romance,romance,lovers revenge,Baby,drama,sand,disease,everything,kiss,hand,touch,friends,friends,friends,friends,romance,romance,passion baby,mine,horror,vertigo shtick,window,psycho,friends,la-la,romance,ton amour,je,la-la,la-la,fashion baby,fashion baby,fashion baby</t>
+  </si>
+  <si>
+    <t>lover,money,pieces,MONEY,Damn,honey,mistress,Jag,That,money,money,Baby,k-kisses,money,knees,money,mansion,jet,trips,islands,gifts,honey,honey,honey,k-kisses,honey,honey,honey,mistress,money,honey,knees,baby,pieces,boat,girls,west coast,beach,champagne,things,tender,babe,candle,money,baby,baby,money,money,money,money,money,K-k</t>
+  </si>
+  <si>
+    <t>possibilities,faithlessness,disbelief,possibilities,memories,possibilities,memories,faithlessness,possibilities,memories,memories,disbelief,memories,possibilities,apologies,memories,control</t>
+  </si>
+  <si>
+    <t>Time,thing,part,mind,rhyme,pendulum swings,end,end,thing,clock,window,Things,memory,rhyme,way,mind,everything,life,spite,way,property,times,end,trust,trust,end,end,end,end,memory,everything</t>
+  </si>
+  <si>
+    <t>na na na,mercy,Cause,blood,alibi,farewell,truth,regret,mercy,pain,slate,hands,uncertainty,Na na na,Na na na na,Na na na</t>
+  </si>
+  <si>
+    <t>greed,I'ma,lies,misery,misery,Choke,Sayin,pride,explanations,patience,greed,way,lies,composure,breaking point sound,ego,way,breaking point,failure,right,threat</t>
+  </si>
+  <si>
+    <t>Thoughts,mind,car,head,bus,train,cab,lane,sky,planes,hands,nothing</t>
+  </si>
+  <si>
+    <t>heart,head,body,war,things,door,each other,score,lipstick,body,body,head,baby,tattoo,head,head,body,baby,body,tattoo,breath,baby,tattoo,baby,baby,baby,Baby</t>
+  </si>
+  <si>
+    <t>news,things,nothing,fortune teller,future,crystal ball,mess,fortune teller,things,song,Summer,fortune teller,fortune teller,matter,leaves,seasons,kind,future,TV,mind,dream,baby,American,fortune teller,fortune teller,seasons,matter,leaves,future,fortune teller,fortune teller,fortune teller,questions,answers,future,rivers,feeling,fortune teller,future</t>
+  </si>
+  <si>
+    <t>kid,ego,Jagger Baby,moves,gear,eyes,moves,heart,show,stars,Oh,moves,moves,tongue,moves,moves,tongue,shit,Nothing,car,secret,tongue,baby,Nobody,toe,control,moves,Jagger You,secret,Nobody</t>
+  </si>
+  <si>
+    <t>one,thinking,Ooh,words,freeway,everything,bout,things,words,cause,curb,Man,death,thread,one,one,cause,cause,Ooh,dirt,death,curb,thread,things,road,words,words,things,cause,one,cause,curb,death,dirt,thread,cause,cause,curb,dirt,Ooh</t>
+  </si>
+  <si>
+    <t>chaos,love,eyes,fire,love,heart,mind,plane,toll,heart,cause,choice,front,appetite,best,pressure,everything,things,wings,hips,Cause,fingertips,same</t>
+  </si>
+  <si>
+    <t>lifestyle,track,Keep searching,Life,karmas,stream,Death,Birth,search,stream,strength,tick tick tick tick tick,tick,tick tick tick tick tick tick tock,search,search,deathstyle,tick tick tick tick tick,strength,tick tick tick tick tick tick tock,track,fear,search,lifestyle,worry,hurry,water,deathstyle,talk,tide,side,deathstyle,fear</t>
+  </si>
+  <si>
+    <t>fight,fire,blood,face,eyes,words,No one,man,man,leave,boy,life,truth,No one,No one,No one,No one,No one,No one,Showin</t>
+  </si>
+  <si>
+    <t>Billie Jean,lover,son,head,hearts,kid,one,floor,round,round,floor,kid,eyes,name,movie scene,beauty queen,girls,perfume,round,floor,son,People,scene,mother,floor,round,schemes,law,advice,Cause,truth,plans,side,lie,demand,baby,baby,photo,kid,son,girls,kid,kid,kid,round,floor,Cause,baby,People,lover,lover,room,smell,son,kid,kid,eyes,heart babe</t>
+  </si>
+  <si>
+    <t>Happy,chance,Fallin,fall,love,love,Fallin,gambler,life,love,love,love,love,game,odds,life,times,freedom,hand,side,stars,affair,beginnings,Laughter,love,love,Little,love,love</t>
+  </si>
+  <si>
+    <t>Michael Michael,letter,Dear Michael You,Dear Michael,record,times,more,eyes,tears,letter,letter,fan,envelope,'s,feelings,heart,picture,love,letter,mister postman,ABC,letter,Girl,mister postman</t>
+  </si>
+  <si>
+    <t>victim,man,mind,place,wind,man,man,change,world,mind,ways,kids,streets,winter coat,life,difference,Gonna,look,collar,needs,man soul,bottle top,summer disregard,each other,ways,willow,message,place,mirror,look,change,message,message,Change,message,wind,change,mirror,mirror,look,look,change,Change,mirror,love,nowhere,kind,world,world,change,Change,world,wind,mirror,change,change,change,change,home,nickel,loan,heart,somebody,dream,pattern,mirror,mirror,change,change,message,Cause,change,change,mirror,mirror,look,Hoo,Brother Hoo,world</t>
+  </si>
+  <si>
+    <t>Livin,part,world,people,feelin,room,shoulder,act,madness,life,chance,folks,Gotta,people,Chorus,Cause,one,shelf,town,wall,wall,life,wall,Life,wall,sin,music,party,Life,inhibitions,exhibition,soul,way,Cause,Chorus,rules,rules,way</t>
+  </si>
+  <si>
+    <t>Cos,face,state,state,knees,baby,style,state,state,shock,Ow Wow Ow,Gotta,Wow Uh,baby,baby,state,state,state,state,state,state,shock,shock,shock,shock,knees,baby,baby,face,baby talk,nah Nah,way,Everybody,Wow Nah,Ow,Na,Talk,state,state,state,shock,shock,shock,shock,state,state,state,da,shock,shock,shock,Yeah,Da, da, da, da, da, da Da, da, da, da, da, da, wow Da, da, da, da, da, da Da, da, da, da, da</t>
+  </si>
+  <si>
+    <t>fireflies,pride,stars,everyone,sky,satellites,trees,Singing Amen,nobody,nobody,nobody,everyone,everyone,everyone,Amen I,pride,nobody,nobody,everyone,nobody,nobody,nobody,nobody,everyone,everyone,pride,everyone,everyone,Amen I,air,paradise,light,Singing Amen,everyone,Amen I,everyone,world,nobody,nobody,nobody,nobody,everyone,nobody,nobody,everyone,nobody,nobody,nobody,world,everyone,everyone,stars</t>
+  </si>
+  <si>
+    <t>eyes,heart,hands,life,mind,heart,heart,mind,mind</t>
+  </si>
+  <si>
+    <t>star,rock stars,way,Hey,house,VIP,bars,cars,life,hair,clubs,king size tub,Cribs,episode,bathroom,ninth,bottom,line,limit,hair,Playboy bunny,rooms,dictionary,tassels,baseball,centerfold,songs,gold digger,credit card,money,rock star,drugs,movie stars,life,drugs,fame,fortune,girls,girls,guitars,jet,bedroom,fashion,club,bleach blond hair,cause,Cause,hilltop houses,drugs,cause,door,Playboy bunny,hilltop houses,songs,name,girls,life,rock star,rock star,Gonna,name,fortune,fame,mansion,meals,ass,quesadilla,tour bus,cause,body guards,hilltop houses,movie stars,Hollywood Boulevard Somewhere,Cher,James Dean,singers,Playboy,rock star,rock star,censors,pills,dispenser,Lip sync,assholes,Elvis,movie stars,anything,Everybody,smile,drug dealer,speed dial,anything,Pez,drug dealer,smile,Everybody,speed dial</t>
+  </si>
+  <si>
+    <t>God,bullet,life,life,little,side,Uncle Sam,name,rage,stage,trigger,brother,world,world,right,bullet,bullet,somebody,world,somebody,hate,home,right,many,bullet,wake,mistake,lives,somebody,right,hate,bullet,bullet,bullet,bullet,home,somebody,hate,home,excuse</t>
+  </si>
+  <si>
+    <t>Chorus,Chorus,eyes,photograph,dollar,Kim,cops,hell,head,owner,Joey,record,floor,things,Lot,school,Most,photo,somebody,door,memory,bye,back door,bedroom floor,memory,bye,photo album,lookin,friend,sneakin,faces,town,kids,God,Oh,photograph,Chorus,thing,arcade,Oh,couple,steering wheel,song,radio</t>
+  </si>
+  <si>
+    <t>something,some,baby,way,way,cradle,something,ripple,Search,way,way,justice,water,stone,way,way,means,end</t>
+  </si>
+  <si>
+    <t>lady,head,whiskey,all,grin,preacher,thread,voice,demons,case,bottle,few,fiddle,Hanging,sister sin,paper,wagon,wheel,case,thread,voice,kind,mud,face,bottle,case,kingdom,bottle,mud,Lying,grace,judge</t>
+  </si>
+  <si>
+    <t>everything,bout,bout,Cool Breeze,crib,face,cause,girl,bout,Breeze,shit,crib,man,Bill Clampett,money,Dimensions,nigga,folks,throat,player card,Big Time,folks,Lexus,thing,Benzo,Big Slate,bout,somebody,bitch,Man,keys,job,sister,Niggas,warehouse,mouth,shit,pimp shit,hemp shit,girl,Decatur,ass,men,loss,crib,bout yo,dime,man,coward,partner,walk,dimwit,Slick,spirits,beat,bodies,warrant,police,Big Boi,baby daddy,quote,home,ignition,Penny pinchers,Buying,mix,White House,Red Dog,Ca,everybody,peers,fuck,fields,shade tree ass ways,fade,hair drag,Great Hoe Round Up Yo,police,Diamond,Coco Grier Ai,East Pointe,Fleetwood,bitch,see-saw,dad,lines,plot,nothing bout,Big Gipp,baby,accidents,corner,highways,ones,sky,dipping,Jumping Lily,Goodie,Sixteen</t>
+  </si>
+  <si>
+    <t>baby,feeling,Nothing,thought,sho,tha door,neighbor,denial,Mom and Dad,God,Yea,Ice cold,Ice cold,exception,daddy,caddy,momma,fellas,feelings,picture,picture,suga,picture,Beyonce,tha floor,tha floor,baby dolls,Polaroid,Lucy Lu,Yea,nothin,thang,thang,sugar,ladies,badest behavior</t>
+  </si>
+  <si>
+    <t>way,Wanda,hurdle,some,Something,situation,introduction,In Living Colors Wanda,ass,everybody,everything,victim,Pocketbook,resort,cash,risk,path,dollar heels,obstacle,things,ass,sarge,bratwurst,pockets,somebody,wife,things,Trick,Fast,life,designer bag,refrigerator,stomach,knot,need,chances,dignity,sacrifice,nothing,knob,yard,massage,job,action,silver locket,reaction,deal,sex,Corvette,man,night stand,knock,Honda,shit,glass door,lick,pockets,wife,tricks,yo,license,Pick</t>
+  </si>
+  <si>
+    <t>friend,idea,Soldiers,eye,rain,horn,tsunamis,storm,Gabriel,friend,Chorus,mind,ride,nick,hurricane,friends,ass soldiers,Soldiers,peace,mind,people,war,voice,boy,girl,wars,mysteries,way,paradise,know,means,mine,Chorus,mine,Bridge,child,way,Bridge,prophecy</t>
+  </si>
+  <si>
+    <t>head,baby blue,dont,babies,baby crawl baby,Miss lady,veiw,repeat,house,Miss lady,baby crawl baby,way,life,type,hairs,hea,couple,sposed,juice,baby,baby,babies,veiw,baby blue,lady,Claire Huxtible,baby talk,dont</t>
+  </si>
+  <si>
+    <t>outkast,someone,system,homeless,society,life,Outkast,outkast,american,Adjective,Operatin,nigga,Tamperin,muzik,truths,principles,cracker,outkast,part,cracker,world,cadillac do,hoes,clothes,beliefs,hair,occupation,anything,skin color,niggaz,food,engineering control,existance,punk,death,fakers,Poisonin,ciggarettes Disease,world,fact,matter,Peace</t>
+  </si>
+  <si>
+    <t>things,things,Somebody,All,things,fun,head,sand,Things,way</t>
+  </si>
+  <si>
+    <t>people,summer sound,land,hand</t>
+  </si>
+  <si>
+    <t>Something,place,head,songs,walk,friend,change,Life,grace,freedom,world,baby,world,soul,baby,make,price,change,Life,change,spirit,freedom,grace,Life,freedom,songs,grace,o' clock,Praise Praise It</t>
+  </si>
+  <si>
+    <t>change,Love,chance,feelings,baby,baby,love,love,friends,Stand up,turn,baby,daylight,dreams,heads,opportunity,love,dreams,love,someone,Want,Ooh,baby,love,love</t>
+  </si>
+  <si>
+    <t>Well,eternity,edge,Cause,love,love,nothin,Wolf tickets,Know,kiss,edge,eternity,edge,edge,eternity,Know,Gettin,thing,Well wait,sky,eternity Pie,Repeat,head spin,it Girl,kiss,Know,edge,edge,edge,edge,ounce,Girl,store,plenty,need</t>
+  </si>
+  <si>
+    <t>veteran,Vietnam,man,war,reason,cost,movie,army,man,man,leg,quote form,jungle,man,hooker,Chorus,front line,front line,line,front line,life,life,back,another,gun,shoot,hand,thrill,kind,urge,pill,uniform,price,friend,head,church,war,mind,lives,junkie,bout,right,Back,purple heart,neighborhood,fear,agent orange,no one,war,nephew,paper,families,brewing,world</t>
+  </si>
+  <si>
+    <t>sight,reality,eyes,eyes,things,Cause,temptation,satisfaction,reality,eyes,Come on girl,reality,eyes,eyes,things,words,way,tradition,someone,reality,baby,Gotta,reality,reality,Gotta,baby,baby,Repeat,reality,things,Cause,disappointment,Repeat,feelings,light,senses,Plus</t>
+  </si>
+  <si>
+    <t>Music,people,people,record,all,world,groove,Basie,band,language,opportunity,dance,hands,people,way,things,people,people,people,groove,letter,people,people,music,one,pioneers,voice,Sir Duke,king,life,some,Ella,Sachmo,Miller,people,people,let</t>
+  </si>
+  <si>
+    <t>baby,cause,Breakin,sweat Cause,man,lovers,love,door,life,dues,boy,man,way,difference,way,man,shock,tears,body,baby,baby,baby,way,love,times,way,Goodbye,way,baby,baby,man,best,baby girl,knees,plea</t>
+  </si>
+  <si>
+    <t>love,Boy,love,one,Londie,love,angel,heaven,meaning,life,love,God,Life,love,Aisha The</t>
+  </si>
+  <si>
+    <t>love,folks,bushes,Some,friend,love,bushes,friend,love,mine,thing,man,mine,heart,mine,Keep,Keep,folks,folks,Cause,end,folks,baby</t>
+  </si>
+  <si>
+    <t>friend,girlfriend,IQ,shortcomings,points,Waiting for Mrs. Right You,perfection,nothing,pain,Foot Hot Look All American Man Sad,Devotion Waiting,concerns,stubbornness</t>
+  </si>
+  <si>
+    <t>arms,girl,knees,charms,girl,girl,knees,mind,Confrontations,air,kiss,feet,Anything,heart,girl,knees,Confrontations,heart,Gods,mind,heart</t>
+  </si>
+  <si>
+    <t>things,cause,dark,mountain,sea,cause,home,Cold</t>
+  </si>
+  <si>
+    <t>friend,house,girl,friend,distance,things,Solo</t>
+  </si>
+  <si>
+    <t>thing,automobile,fashion sense,Livin,way,Beverly Hills Beverly Hills,crap,friends,girls,boarding schools,nobody,Preppie,pocket,celebrity,picture,movie stars,life,nothing,housemaids,pool,Cause,king,floors,spaces,life,stars,livin,celebrity,Beverly Hills Look,Beverly Hills Beverly Hills,fool,truth,chance</t>
+  </si>
+  <si>
+    <t>Everybody,some,games,cow,friends,fun,cows,baseball bat,Everybody,fences,hits,eggs,Toilet paper,mail boxes,bit,Everybody,Everybody,Everybody,damage,practice,benches,chairs,tables,Lookin,kids,way,Causin,knives,knives,nighttimes,road kills,ponds,forces,corpses,thrills,fire,things,safety pads,guardian angel,confession,friend,paths,destiny,kind,Lightin,Hockey,smile,face,Cause,place,ninja swords,country roads,keys,wheel,parents,zone,home,Hey Dad,Tercel,Drivin</t>
+  </si>
+  <si>
+    <t>times,games,sun</t>
+  </si>
+  <si>
+    <t>king,baby,thing,dude,slack,biz,disco,beer Act,army,losers,respect,babies,something,something,Some,some,town,kick,attention,something,action,winners,man,something,Nobody,biz,town,Life</t>
+  </si>
+  <si>
+    <t>heart,Cause,baby,baby,love,heart,everybody,baby,baby,stars,photograph,photograph,everybody,Something,photograph,photograph,photograph,place,hope,love,oo-oo-oo,baby,baby,photograph,heart,love,everybody,Something,dream,plans</t>
+  </si>
+  <si>
+    <t>water slide,life taker,Somebody,icebox,cold one,Alright Somebody's Heine' Is crowdin,chills,Wrestle,life taker,stepfather,bottle,drug,back,drug,love,way,Jimmy Something,eyes,Inside Flip,bottle,drug,feelings,son,flood,heart breaker,heart breaker,Steven,life taker,Daddy,silence,things,heart breaker,Jesus</t>
+  </si>
+  <si>
+    <t>motherfuckers,motherfuckers,rap,Wu-Tang Incorp,addition,niggas,motherfuckers,Wu,world,compositions,disaster,paint,rap star twinkle killer instinct,parables,LP,missions,turf,match,industry,underground,style,Scattin,Earth Wicked,look,Bitch ass niggaz,walkin,skunk,feet,compartments,dart,head,wall,bitches,trunk,monk,mural,tree top,funk,advantage,garment,manifestation,rituals,coal,Wright Brothers,dirt,Iron Lung,world,skunk,name,touch,chunk,words,Jim Thorpe,Hard,Rhymin,Ya,Moonshine,carnage,momma,motherfuckers,bitch,fuss,nigga,frisbee,wall,brain,sink box,Stink box,fuse,lunch,church,doves,bus,news,Gold,booze,grandfather,mouth,cook-out,fuck,man,plane,funny bone tickler,murder rap,dick sex enigma pistol,stigma,order,get,ink blots,spacewalk,directors,dosage,notice,postage,Dirty,Bitch,RZA Yo,Attack,flow,destruction,production,trust nothin,somethin,dart gun,bustin,angle,code,homage,bout,nose,Zig-Zag-Zig A,bals,Unglove,The Indian,Manhattan,Caligula,The Riddler,line,MC,B-jork,screamin,Be,target,rock,drill sergeant,crew,sundial,point,Jesus,Twisted Metal,Agent Orange,yo,feet,rap souflee saute,hands,plague,jig,proof,goose,fetus,copies,noose,cranberry fruit juice Ginseng boost,money,bar nickle,Drunk,Su,Wu Thirty-Six,Chambers,neck,egg,Absolut,Leg Leg Arm,Eighty,Hennessee,Kinko</t>
+  </si>
+  <si>
+    <t>H-O-D,Comin,method man,cloud,style,Shaolin,slums,jam,H-O-D,H-O-D,Method Man,Method Man Straight,MAN M-E-T,MAN M-E-T,MAN Hey,White Owls,Ghost Face Killer,Inspecktah Deck,Ol Dirty Bastard,GZA,God,Raekwon the Chef You,RZA,Wu-Tang Fading,Humpty Hump Wow,Style,butter,Method Man,meth,jam,cause,cake patty cake,eggs,angle,Upside downside,ham,fact,rubber Band,flam,Sam Sam I am,doubt,commotion,shit,some,some,skins,skin,coast,diggy dog shit,putty tat,behavior savior,Peter Pan Peanut butter,All,paw,poetry,plan,master,corn,lord,sword,skunk,bags,lotion,motion,licks,flavor,pantie raider,forty,shorty,huff,snow,blowin,wind,mic,Question,Hittin,Skippy,Jif,flow,Child,boom,no one,crews,motherfuckers,crew,isle,bleach,glass,center,break Peep,Saran Wrap,Method All,soul,Like Deck,song,sperm,man,Fat Albert,Method,MAN,Ill,Zoom,cause,slums,mother,posse,friends,swarm,chambers,death,kid,Word,peace,Chim chimmeny chim chim cherie Freak,Tootsie Roll,flow,butt,girls rumps,sex,things,hoes,bitch squirm,ballistics Missiles,game,pistol Clip,slug,jump,brain,pump,Wu-Tang Killa Bee,Super Sperm,Yo,Joe</t>
+  </si>
+  <si>
+    <t>Man,radio station,Fiends,world,world,God,world,man,shit,baby,hip-hop shit,mothers,death,MC,Damn,hill,Wu-Tang Wu-Tang,jiggy,mind,stress,enslavement,project pavement,hip-hop game,step,world,LP,world,Lord,window,sky,dark,hip-hop game,project pavement,enslavement,mind,stress,train,melody,ear,tape,hip-hop game,same,pain,tape,sky,dark,window,sign,knowledge,air,Billboards</t>
+  </si>
+  <si>
+    <t>Google_Entities_Tentative</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2250,7 +2630,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2273,13 +2653,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2288,6 +2682,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2334,7 +2736,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2366,9 +2768,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2400,6 +2820,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2575,14 +3013,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M124"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2619,8 +3059,14 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2660,8 +3106,14 @@
       <c r="M2" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2" t="s">
+        <v>736</v>
+      </c>
+      <c r="O2">
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2701,8 +3153,14 @@
       <c r="M3" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3" t="s">
+        <v>737</v>
+      </c>
+      <c r="O3">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2742,8 +3200,14 @@
       <c r="M4" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4" t="s">
+        <v>738</v>
+      </c>
+      <c r="O4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2783,8 +3247,14 @@
       <c r="M5" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5" t="s">
+        <v>739</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2824,8 +3294,14 @@
       <c r="M6" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6" t="s">
+        <v>740</v>
+      </c>
+      <c r="O6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2865,8 +3341,14 @@
       <c r="M7" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7" t="s">
+        <v>741</v>
+      </c>
+      <c r="O7">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2906,8 +3388,14 @@
       <c r="M8" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8" t="s">
+        <v>742</v>
+      </c>
+      <c r="O8">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2947,8 +3435,14 @@
       <c r="M9" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9" t="s">
+        <v>743</v>
+      </c>
+      <c r="O9">
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2988,8 +3482,14 @@
       <c r="M10" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10" t="s">
+        <v>744</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3029,8 +3529,14 @@
       <c r="M11" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11" t="s">
+        <v>745</v>
+      </c>
+      <c r="O11">
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3070,8 +3576,14 @@
       <c r="M12" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="N12" t="s">
+        <v>746</v>
+      </c>
+      <c r="O12">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3111,8 +3623,14 @@
       <c r="M13" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="N13" t="s">
+        <v>747</v>
+      </c>
+      <c r="O13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3152,8 +3670,14 @@
       <c r="M14" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14" t="s">
+        <v>748</v>
+      </c>
+      <c r="O14">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3193,8 +3717,14 @@
       <c r="M15" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="N15" t="s">
+        <v>749</v>
+      </c>
+      <c r="O15">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3234,8 +3764,14 @@
       <c r="M16" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16" t="s">
+        <v>750</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -3275,8 +3811,14 @@
       <c r="M17" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17" t="s">
+        <v>751</v>
+      </c>
+      <c r="O17">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -3316,8 +3858,14 @@
       <c r="M18" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18" t="s">
+        <v>752</v>
+      </c>
+      <c r="O18">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -3357,8 +3905,14 @@
       <c r="M19" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19" t="s">
+        <v>753</v>
+      </c>
+      <c r="O19">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -3398,8 +3952,14 @@
       <c r="M20" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20" t="s">
+        <v>754</v>
+      </c>
+      <c r="O20">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -3439,8 +3999,14 @@
       <c r="M21" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21" t="s">
+        <v>755</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -3480,8 +4046,14 @@
       <c r="M22" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="N22" t="s">
+        <v>756</v>
+      </c>
+      <c r="O22">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -3521,8 +4093,14 @@
       <c r="M23" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="N23" t="s">
+        <v>757</v>
+      </c>
+      <c r="O23">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -3562,8 +4140,14 @@
       <c r="M24" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="N24" t="s">
+        <v>758</v>
+      </c>
+      <c r="O24">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -3600,8 +4184,14 @@
       <c r="M25" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="N25" t="s">
+        <v>759</v>
+      </c>
+      <c r="O25">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -3641,8 +4231,14 @@
       <c r="M26" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="N26" t="s">
+        <v>760</v>
+      </c>
+      <c r="O26">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -3682,8 +4278,14 @@
       <c r="M27" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="N27" t="s">
+        <v>761</v>
+      </c>
+      <c r="O27">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -3723,8 +4325,14 @@
       <c r="M28" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="N28" t="s">
+        <v>762</v>
+      </c>
+      <c r="O28">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -3764,8 +4372,14 @@
       <c r="M29" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="N29" t="s">
+        <v>763</v>
+      </c>
+      <c r="O29">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -3805,8 +4419,14 @@
       <c r="M30" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="N30" t="s">
+        <v>764</v>
+      </c>
+      <c r="O30">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3846,8 +4466,14 @@
       <c r="M31" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="N31" t="s">
+        <v>765</v>
+      </c>
+      <c r="O31">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3884,8 +4510,14 @@
       <c r="M32" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="N32" t="s">
+        <v>766</v>
+      </c>
+      <c r="O32">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3925,8 +4557,14 @@
       <c r="M33" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="N33" t="s">
+        <v>767</v>
+      </c>
+      <c r="O33">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3966,8 +4604,14 @@
       <c r="M34" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="N34" t="s">
+        <v>768</v>
+      </c>
+      <c r="O34">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -4007,8 +4651,14 @@
       <c r="M35" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="N35" t="s">
+        <v>769</v>
+      </c>
+      <c r="O35">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -4048,8 +4698,14 @@
       <c r="M36" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="N36" t="s">
+        <v>770</v>
+      </c>
+      <c r="O36">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -4089,8 +4745,14 @@
       <c r="M37" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="N37" t="s">
+        <v>771</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -4130,8 +4792,14 @@
       <c r="M38" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="N38" t="s">
+        <v>772</v>
+      </c>
+      <c r="O38">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -4171,8 +4839,14 @@
       <c r="M39" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="N39" t="s">
+        <v>773</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -4212,8 +4886,14 @@
       <c r="M40" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="N40" t="s">
+        <v>774</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -4253,8 +4933,14 @@
       <c r="M41" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="42" spans="1:13">
+      <c r="N41" t="s">
+        <v>775</v>
+      </c>
+      <c r="O41">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -4294,8 +4980,14 @@
       <c r="M42" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="N42" t="s">
+        <v>776</v>
+      </c>
+      <c r="O42">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -4335,8 +5027,14 @@
       <c r="M43" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="44" spans="1:13">
+      <c r="N43" t="s">
+        <v>777</v>
+      </c>
+      <c r="O43">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -4373,8 +5071,14 @@
       <c r="M44" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="N44" t="s">
+        <v>778</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -4414,8 +5118,14 @@
       <c r="M45" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="46" spans="1:13">
+      <c r="N45" t="s">
+        <v>779</v>
+      </c>
+      <c r="O45">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -4455,8 +5165,14 @@
       <c r="M46" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="47" spans="1:13">
+      <c r="N46" t="s">
+        <v>780</v>
+      </c>
+      <c r="O46">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -4496,8 +5212,14 @@
       <c r="M47" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="N47" t="s">
+        <v>781</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -4537,8 +5259,14 @@
       <c r="M48" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="N48" t="s">
+        <v>782</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4578,8 +5306,14 @@
       <c r="M49" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="N49" t="s">
+        <v>783</v>
+      </c>
+      <c r="O49">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -4619,8 +5353,14 @@
       <c r="M50" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="51" spans="1:13">
+      <c r="N50" t="s">
+        <v>784</v>
+      </c>
+      <c r="O50">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -4660,8 +5400,14 @@
       <c r="M51" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="N51" t="s">
+        <v>785</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -4701,8 +5447,14 @@
       <c r="M52" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="N52" t="s">
+        <v>786</v>
+      </c>
+      <c r="O52">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -4742,8 +5494,14 @@
       <c r="M53" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="N53" t="s">
+        <v>787</v>
+      </c>
+      <c r="O53">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -4783,8 +5541,14 @@
       <c r="M54" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="N54" t="s">
+        <v>788</v>
+      </c>
+      <c r="O54">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -4824,8 +5588,14 @@
       <c r="M55" t="s">
         <v>666</v>
       </c>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="N55" t="s">
+        <v>789</v>
+      </c>
+      <c r="O55">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -4865,8 +5635,14 @@
       <c r="M56" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="57" spans="1:13">
+      <c r="N56" t="s">
+        <v>790</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -4906,8 +5682,14 @@
       <c r="M57" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="N57" t="s">
+        <v>791</v>
+      </c>
+      <c r="O57">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -4947,8 +5729,14 @@
       <c r="M58" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="59" spans="1:13">
+      <c r="N58" t="s">
+        <v>792</v>
+      </c>
+      <c r="O58">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -4985,8 +5773,14 @@
       <c r="M59" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="N59" t="s">
+        <v>793</v>
+      </c>
+      <c r="O59">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -5026,8 +5820,14 @@
       <c r="M60" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="61" spans="1:13">
+      <c r="N60" t="s">
+        <v>794</v>
+      </c>
+      <c r="O60">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -5067,8 +5867,14 @@
       <c r="M61" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="62" spans="1:13">
+      <c r="N61" t="s">
+        <v>795</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -5108,8 +5914,14 @@
       <c r="M62" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="63" spans="1:13">
+      <c r="N62" t="s">
+        <v>796</v>
+      </c>
+      <c r="O62">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -5149,8 +5961,14 @@
       <c r="M63" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="64" spans="1:13">
+      <c r="N63" t="s">
+        <v>797</v>
+      </c>
+      <c r="O63">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -5190,8 +6008,14 @@
       <c r="M64" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="65" spans="1:13">
+      <c r="N64" t="s">
+        <v>798</v>
+      </c>
+      <c r="O64">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -5231,8 +6055,14 @@
       <c r="M65" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="66" spans="1:13">
+      <c r="N65" t="s">
+        <v>799</v>
+      </c>
+      <c r="O65">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -5272,8 +6102,14 @@
       <c r="M66" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="67" spans="1:13">
+      <c r="N66" t="s">
+        <v>800</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -5313,8 +6149,14 @@
       <c r="M67" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="68" spans="1:13">
+      <c r="N67" t="s">
+        <v>801</v>
+      </c>
+      <c r="O67">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -5354,8 +6196,14 @@
       <c r="M68" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="69" spans="1:13">
+      <c r="N68" t="s">
+        <v>802</v>
+      </c>
+      <c r="O68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -5395,8 +6243,14 @@
       <c r="M69" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="70" spans="1:13">
+      <c r="N69" t="s">
+        <v>803</v>
+      </c>
+      <c r="O69">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -5436,8 +6290,14 @@
       <c r="M70" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="71" spans="1:13">
+      <c r="N70" t="s">
+        <v>804</v>
+      </c>
+      <c r="O70">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -5477,8 +6337,14 @@
       <c r="M71" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="72" spans="1:13">
+      <c r="N71" t="s">
+        <v>805</v>
+      </c>
+      <c r="O71">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -5518,8 +6384,14 @@
       <c r="M72" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="73" spans="1:13">
+      <c r="N72" t="s">
+        <v>806</v>
+      </c>
+      <c r="O72">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -5559,8 +6431,14 @@
       <c r="M73" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="74" spans="1:13">
+      <c r="N73" t="s">
+        <v>807</v>
+      </c>
+      <c r="O73">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -5600,8 +6478,14 @@
       <c r="M74" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="75" spans="1:13">
+      <c r="N74" t="s">
+        <v>808</v>
+      </c>
+      <c r="O74">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -5641,8 +6525,14 @@
       <c r="M75" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="76" spans="1:13">
+      <c r="N75" t="s">
+        <v>809</v>
+      </c>
+      <c r="O75">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -5682,8 +6572,14 @@
       <c r="M76" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="77" spans="1:13">
+      <c r="N76" t="s">
+        <v>810</v>
+      </c>
+      <c r="O76">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -5723,8 +6619,14 @@
       <c r="M77" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="78" spans="1:13">
+      <c r="N77" t="s">
+        <v>811</v>
+      </c>
+      <c r="O77">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -5764,8 +6666,14 @@
       <c r="M78" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="79" spans="1:13">
+      <c r="N78" t="s">
+        <v>812</v>
+      </c>
+      <c r="O78">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -5805,8 +6713,14 @@
       <c r="M79" t="s">
         <v>690</v>
       </c>
-    </row>
-    <row r="80" spans="1:13">
+      <c r="N79" t="s">
+        <v>813</v>
+      </c>
+      <c r="O79">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -5846,8 +6760,14 @@
       <c r="M80" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="81" spans="1:13">
+      <c r="N80" t="s">
+        <v>814</v>
+      </c>
+      <c r="O80">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -5887,8 +6807,14 @@
       <c r="M81" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="82" spans="1:13">
+      <c r="N81" t="s">
+        <v>815</v>
+      </c>
+      <c r="O81">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -5928,8 +6854,14 @@
       <c r="M82" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="83" spans="1:13">
+      <c r="N82" t="s">
+        <v>816</v>
+      </c>
+      <c r="O82">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -5969,8 +6901,14 @@
       <c r="M83" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="84" spans="1:13">
+      <c r="N83" t="s">
+        <v>817</v>
+      </c>
+      <c r="O83">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -6010,8 +6948,14 @@
       <c r="M84" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="85" spans="1:13">
+      <c r="N84" t="s">
+        <v>818</v>
+      </c>
+      <c r="O84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -6051,8 +6995,14 @@
       <c r="M85" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="86" spans="1:13">
+      <c r="N85" t="s">
+        <v>819</v>
+      </c>
+      <c r="O85">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -6092,8 +7042,14 @@
       <c r="M86" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="87" spans="1:13">
+      <c r="N86" t="s">
+        <v>820</v>
+      </c>
+      <c r="O86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -6133,8 +7089,14 @@
       <c r="M87" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="88" spans="1:13">
+      <c r="N87" t="s">
+        <v>821</v>
+      </c>
+      <c r="O87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -6174,8 +7136,14 @@
       <c r="M88" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="89" spans="1:13">
+      <c r="N88" t="s">
+        <v>822</v>
+      </c>
+      <c r="O88">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -6212,8 +7180,14 @@
       <c r="M89" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="90" spans="1:13">
+      <c r="N89" t="s">
+        <v>823</v>
+      </c>
+      <c r="O89">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -6253,8 +7227,14 @@
       <c r="M90" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="91" spans="1:13">
+      <c r="N90" t="s">
+        <v>824</v>
+      </c>
+      <c r="O90">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -6294,8 +7274,14 @@
       <c r="M91" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="92" spans="1:13">
+      <c r="N91" t="s">
+        <v>825</v>
+      </c>
+      <c r="O91">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -6335,8 +7321,14 @@
       <c r="M92" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="93" spans="1:13">
+      <c r="N92" t="s">
+        <v>826</v>
+      </c>
+      <c r="O92">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -6373,8 +7365,14 @@
       <c r="M93" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="94" spans="1:13">
+      <c r="N93" t="s">
+        <v>827</v>
+      </c>
+      <c r="O93">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -6414,8 +7412,14 @@
       <c r="M94" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="95" spans="1:13">
+      <c r="N94" t="s">
+        <v>828</v>
+      </c>
+      <c r="O94">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -6455,8 +7459,14 @@
       <c r="M95" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="96" spans="1:13">
+      <c r="N95" t="s">
+        <v>829</v>
+      </c>
+      <c r="O95">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -6496,8 +7506,14 @@
       <c r="M96" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="97" spans="1:13">
+      <c r="N96" t="s">
+        <v>830</v>
+      </c>
+      <c r="O96">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -6537,8 +7553,14 @@
       <c r="M97" t="s">
         <v>707</v>
       </c>
-    </row>
-    <row r="98" spans="1:13">
+      <c r="N97" t="s">
+        <v>831</v>
+      </c>
+      <c r="O97">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -6578,8 +7600,14 @@
       <c r="M98" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="99" spans="1:13">
+      <c r="N98" t="s">
+        <v>832</v>
+      </c>
+      <c r="O98">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -6619,8 +7647,14 @@
       <c r="M99" t="s">
         <v>709</v>
       </c>
-    </row>
-    <row r="100" spans="1:13">
+      <c r="N99" t="s">
+        <v>833</v>
+      </c>
+      <c r="O99">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -6660,8 +7694,14 @@
       <c r="M100" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="101" spans="1:13">
+      <c r="N100" t="s">
+        <v>834</v>
+      </c>
+      <c r="O100">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -6698,8 +7738,14 @@
       <c r="M101" t="s">
         <v>711</v>
       </c>
-    </row>
-    <row r="102" spans="1:13">
+      <c r="N101" t="s">
+        <v>835</v>
+      </c>
+      <c r="O101">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -6736,8 +7782,14 @@
       <c r="M102" t="s">
         <v>712</v>
       </c>
-    </row>
-    <row r="103" spans="1:13">
+      <c r="N102" t="s">
+        <v>836</v>
+      </c>
+      <c r="O102">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -6777,8 +7829,14 @@
       <c r="M103" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="104" spans="1:13">
+      <c r="N103" t="s">
+        <v>837</v>
+      </c>
+      <c r="O103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -6818,8 +7876,14 @@
       <c r="M104" t="s">
         <v>714</v>
       </c>
-    </row>
-    <row r="105" spans="1:13">
+      <c r="N104" t="s">
+        <v>838</v>
+      </c>
+      <c r="O104">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -6859,8 +7923,14 @@
       <c r="M105" t="s">
         <v>715</v>
       </c>
-    </row>
-    <row r="106" spans="1:13">
+      <c r="N105" t="s">
+        <v>839</v>
+      </c>
+      <c r="O105">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -6900,8 +7970,14 @@
       <c r="M106" t="s">
         <v>716</v>
       </c>
-    </row>
-    <row r="107" spans="1:13">
+      <c r="N106" t="s">
+        <v>840</v>
+      </c>
+      <c r="O106">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -6941,8 +8017,14 @@
       <c r="M107" t="s">
         <v>717</v>
       </c>
-    </row>
-    <row r="108" spans="1:13">
+      <c r="N107" t="s">
+        <v>841</v>
+      </c>
+      <c r="O107">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -6982,8 +8064,14 @@
       <c r="M108" t="s">
         <v>718</v>
       </c>
-    </row>
-    <row r="109" spans="1:13">
+      <c r="N108" t="s">
+        <v>842</v>
+      </c>
+      <c r="O108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -7023,8 +8111,14 @@
       <c r="M109" t="s">
         <v>719</v>
       </c>
-    </row>
-    <row r="110" spans="1:13">
+      <c r="N109" t="s">
+        <v>843</v>
+      </c>
+      <c r="O109">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -7064,8 +8158,14 @@
       <c r="M110" t="s">
         <v>720</v>
       </c>
-    </row>
-    <row r="111" spans="1:13">
+      <c r="N110" t="s">
+        <v>844</v>
+      </c>
+      <c r="O110">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -7102,8 +8202,14 @@
       <c r="M111" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="112" spans="1:13">
+      <c r="N111" t="s">
+        <v>845</v>
+      </c>
+      <c r="O111">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -7143,8 +8249,14 @@
       <c r="M112" t="s">
         <v>722</v>
       </c>
-    </row>
-    <row r="113" spans="1:13">
+      <c r="N112" t="s">
+        <v>846</v>
+      </c>
+      <c r="O112">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -7184,8 +8296,14 @@
       <c r="M113" t="s">
         <v>723</v>
       </c>
-    </row>
-    <row r="114" spans="1:13">
+      <c r="N113" t="s">
+        <v>847</v>
+      </c>
+      <c r="O113">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -7222,8 +8340,14 @@
       <c r="M114" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="115" spans="1:13">
+      <c r="N114" t="s">
+        <v>848</v>
+      </c>
+      <c r="O114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -7263,8 +8387,14 @@
       <c r="M115" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="116" spans="1:13">
+      <c r="N115" t="s">
+        <v>849</v>
+      </c>
+      <c r="O115">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -7304,8 +8434,14 @@
       <c r="M116" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="117" spans="1:13">
+      <c r="N116" t="s">
+        <v>850</v>
+      </c>
+      <c r="O116">
+        <v>-0.7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -7345,8 +8481,14 @@
       <c r="M117" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="118" spans="1:13">
+      <c r="N117" t="s">
+        <v>851</v>
+      </c>
+      <c r="O117">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -7386,8 +8528,14 @@
       <c r="M118" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="119" spans="1:13">
+      <c r="N118" t="s">
+        <v>852</v>
+      </c>
+      <c r="O118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -7427,8 +8575,14 @@
       <c r="M119" t="s">
         <v>729</v>
       </c>
-    </row>
-    <row r="120" spans="1:13">
+      <c r="N119" t="s">
+        <v>853</v>
+      </c>
+      <c r="O119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -7468,8 +8622,14 @@
       <c r="M120" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="121" spans="1:13">
+      <c r="N120" t="s">
+        <v>854</v>
+      </c>
+      <c r="O120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -7509,8 +8669,14 @@
       <c r="M121" t="s">
         <v>731</v>
       </c>
-    </row>
-    <row r="122" spans="1:13">
+      <c r="N121" t="s">
+        <v>855</v>
+      </c>
+      <c r="O121">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -7550,8 +8716,14 @@
       <c r="M122" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="123" spans="1:13">
+      <c r="N122" t="s">
+        <v>856</v>
+      </c>
+      <c r="O122">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -7591,8 +8763,14 @@
       <c r="M123" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="124" spans="1:13">
+      <c r="N123" t="s">
+        <v>857</v>
+      </c>
+      <c r="O123">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -7631,6 +8809,12 @@
       </c>
       <c r="M124" t="s">
         <v>734</v>
+      </c>
+      <c r="N124" t="s">
+        <v>858</v>
+      </c>
+      <c r="O124">
+        <v>-0.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>